<commit_message>
got latest timeline file
</commit_message>
<xml_diff>
--- a/almamet-timeline.xlsx
+++ b/almamet-timeline.xlsx
@@ -290,7 +290,7 @@
 </t>
   </si>
   <si>
-    <t>01/06/2018</t>
+    <t>06/01/2018</t>
   </si>
   <si>
     <t>&lt;div class="timeline-title"&gt;Almamet Gmbh- New addition of Desulphurization Technology&lt;/div&gt;</t>
@@ -299,7 +299,7 @@
     <t>&lt;div class="timeline-date"&gt;1st June 2018&lt;/div&gt;Almamet took over metallurgical injection desulphurization technology in Iron and Steel of ThyssenKrupp Ploysius. ThyssenKrupp has commissioned around 130 desulphurization station worldwide since 1963. The technical team from ThyssenKrupp has joined Almamet and the Industrial Solutions office has been set up at Oelde, Germany.</t>
   </si>
   <si>
-    <t>19/06/2018</t>
+    <t>06/19/2018</t>
   </si>
   <si>
     <t>&lt;div class="timeline-title"&gt;Almamet Gmbh – first contract in Desuplhrization technology in India&lt;/div&gt;</t>
@@ -308,13 +308,13 @@
     <t>&lt;div class="timeline-date"&gt;19th June 2018&lt;/div&gt; immediately after becoming a technology supplier, Almamet Gmbh signed its first agreement for supply of engineering and equipment for 250MT *2 twin desulphurization station (co-injection technology) with Jindal Steel and Power (JSPL) for its Angul works.</t>
   </si>
   <si>
-    <t>29/06/2018</t>
+    <t>06/29/2018</t>
   </si>
   <si>
     <t>&lt;div class="timeline-title"&gt;Almamet India – Operation and Maintenance contract for Desulphurization&lt;/div&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;div class="timeline-date"&gt;29thJune 2018&lt;/div&gt; Almamet India signed an agreement for operation and maintenance including supply of reagents and consumables for HMDS facility with Jindal Steel and Power (JSPL) for its Angul works. 
+    <t xml:space="preserve">&lt;div class="timeline-date"&gt;29th June 2018&lt;/div&gt; Almamet India signed an agreement for operation and maintenance including supply of reagents and consumables for HMDS facility with Jindal Steel and Power (JSPL) for its Angul works. 
 This makes Almamet unique as we supply engineering &amp; equipment for HMDS and thereafter also take care of complete operation and maintenance. </t>
   </si>
 </sst>

</xml_diff>

<commit_message>
almamet-timeline.xlsx: removed uncessary caps from content
</commit_message>
<xml_diff>
--- a/almamet-timeline.xlsx
+++ b/almamet-timeline.xlsx
@@ -237,7 +237,7 @@
     <t>&lt;div class="timeline-title"&gt;ALMAMET India 2012 &lt;/div&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;div class="timeline-date"&gt;2012&lt;/div&gt;ALMAMET formed a Joint Venture with an Indian company in 2001 known as ALMAMET Reagents (India) Pvt Ltd. Through this JV ALMAMET was catering to steel plants e.g. TATA, JSW, BHUSHAN, ESSAR &amp; SAIL. ALMAMET also had a production unit of Calcium Carbide blends in Bhilai. In 2012 ALMAMET decides to run its own company by establishing ALMAMET India Private Limited. Since the foundation in 2012 ALMAMET India Private Limited is in discussion with the Indian steel industry to invest in various projects. At the same time ALMAMET India Private Limited is in discussion with companies from chemical &amp; pyrotechnical sector. In near future the ALMAMET group will take major investments to increase the representation within the subcontinent of India. </t>
+    <t xml:space="preserve">&lt;div class="timeline-date"&gt;2012&lt;/div&gt;ALMAMET formed a Joint Venture with an Indian company in 2001 known as ALMAMET Reagents (India) Pvt Ltd. Through this JV ALMAMET was catering to steel plants e.g. TATA, JSW, BHUSHAN, ESSAR &amp; SAIL. ALMAMET also had a production unit of calcium carbide blends in Bhilai. In 2012 ALMAMET decides to run its own company by establishing ALMAMET India Private Limited. Since the foundation in 2012 ALMAMET India Private Limited is in discussion with the Indian steel industry to invest in various projects. At the same time ALMAMET India Private Limited is in discussion with companies from chemical &amp; pyrotechnical sector. In near future the ALMAMET group will take major investments to increase the representation within the subcontinent of India. </t>
   </si>
   <si>
     <t>2013</t>
@@ -260,7 +260,7 @@
 </t>
   </si>
   <si>
-    <t>&lt;div class="timeline-title"&gt;Almamet India Warehouse, Karnataka.&lt;/div&gt;</t>
+    <t>&lt;div class="timeline-title"&gt;Almamet India warehouse, Karnataka.&lt;/div&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -282,27 +282,27 @@
     <t>2018</t>
   </si>
   <si>
-    <t>&lt;div class="timeline-title"&gt;Almamet India Symposium.&lt;/div&gt;</t>
+    <t>&lt;div class="timeline-title"&gt;Almamet India symposium.&lt;/div&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">
-&lt;div class="timeline-date"&gt;2018&lt;/div&gt;Almamet held its First Symposium on Hot Metal Desulphurization in February 2018 in Bhubaneswar.
+&lt;div class="timeline-date"&gt;2018&lt;/div&gt;Almamet held its first symposium on hot metal desulphurization in February 2018 in Bhubaneswar.
 </t>
   </si>
   <si>
     <t>06/01/2018</t>
   </si>
   <si>
-    <t>&lt;div class="timeline-title"&gt;Almamet Gmbh- New addition of Desulphurization Technology&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t>&lt;div class="timeline-date"&gt;1st June 2018&lt;/div&gt;Almamet took over metallurgical injection desulphurization technology in Iron and Steel of ThyssenKrupp Ploysius. ThyssenKrupp has commissioned around 130 desulphurization station worldwide since 1963. The technical team from ThyssenKrupp has joined Almamet and the Industrial Solutions office has been set up at Oelde, Germany.</t>
+    <t>&lt;div class="timeline-title"&gt;Almamet Gmbh- New addition of desulphurization technology&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class="timeline-date"&gt;1st June 2018&lt;/div&gt;Almamet took over metallurgical injection desulphurization technology in iron and steel from ThyssenKrupp Ploysius. ThyssenKrupp has commissioned around 130 desulphurization station worldwide since 1963. The technical team from ThyssenKrupp has joined Almamet and the industrial solutions office has been set up at Oelde, Germany.</t>
   </si>
   <si>
     <t>06/19/2018</t>
   </si>
   <si>
-    <t>&lt;div class="timeline-title"&gt;Almamet Gmbh – first contract in Desuplhrization technology in India&lt;/div&gt;</t>
+    <t>&lt;div class="timeline-title"&gt;Almamet Gmbh – first contract in desuplhrization technology in India&lt;/div&gt;</t>
   </si>
   <si>
     <t>&lt;div class="timeline-date"&gt;19th June 2018&lt;/div&gt; immediately after becoming a technology supplier, Almamet Gmbh signed its first agreement for supply of engineering and equipment for 250MT *2 twin desulphurization station (co-injection technology) with Jindal Steel and Power (JSPL) for its Angul works.</t>
@@ -311,7 +311,7 @@
     <t>06/29/2018</t>
   </si>
   <si>
-    <t>&lt;div class="timeline-title"&gt;Almamet India – Operation and Maintenance contract for Desulphurization&lt;/div&gt;</t>
+    <t>&lt;div class="timeline-title"&gt;Almamet India – Operation and maintenance contract for desulphurization&lt;/div&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;div class="timeline-date"&gt;29th June 2018&lt;/div&gt; Almamet India signed an agreement for operation and maintenance including supply of reagents and consumables for HMDS facility with Jindal Steel and Power (JSPL) for its Angul works. 
@@ -753,7 +753,7 @@
       <c r="C15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="18" t="s">
         <v>51</v>
       </c>
       <c r="E15" s="9"/>

</xml_diff>